<commit_message>
Config file code added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da940c40b94d8f08/Documents/UiPath/Stardex/Challenge20/Challenge20/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da940c40b94d8f08/Documents/UiPath/Stardex/Challenge21/Challenge21/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_B00856F198B06605C11CD1EF960F9E6B0C4A20B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95931A0B-DEE7-466D-8C0B-950AA85BB413}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_B00856F198B06605C11CD1EF960F9E6B0C4A20B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C95C8E6-4300-4C23-83CF-87BC17A32B9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -40,40 +40,22 @@
     <t xml:space="preserve">Pre-Requisite </t>
   </si>
   <si>
-    <t>ProcurementURL</t>
-  </si>
-  <si>
-    <t>https://developer.automationanywhere.com/challenges/AutomationAnywhereLabs-POtrackingLookup.html</t>
-  </si>
-  <si>
-    <t>POURL</t>
-  </si>
-  <si>
-    <t>https://developer.automationanywhere.com/challenges/automationanywherelabs-supplychainmanagement.html</t>
-  </si>
-  <si>
-    <t>LoginUsername</t>
-  </si>
-  <si>
-    <t>Pwd</t>
-  </si>
-  <si>
-    <t>admin@procurementanywhere.com</t>
-  </si>
-  <si>
-    <t>paypacksh!p</t>
-  </si>
-  <si>
-    <t>AgentExcelPath</t>
-  </si>
-  <si>
-    <t>C:\Users\ganes\OneDrive\Documents\UiPath\Stardex\Challenge20\Challenge20\Input</t>
-  </si>
-  <si>
     <t>ConfigFilePath</t>
   </si>
   <si>
-    <t>C:\Users\ganes\OneDrive\Documents\UiPath\Stardex\Challenge20\Challenge20\Data\config.xlsx</t>
+    <t>https://developer.automationanywhere.com/challenges/automationanywherelabs-employeedatamigration.html</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>EndpointURL</t>
+  </si>
+  <si>
+    <t>https://botgames-employee-data-migration-vwsrh7tyda-uc.a.run.app/employees?id=</t>
+  </si>
+  <si>
+    <t>C:\Users\ganes\OneDrive\Documents\UiPath\Stardex\Challenge21\Challenge21\Data\config.xlsx</t>
   </si>
 </sst>
 </file>
@@ -446,11 +428,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -472,7 +452,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -480,55 +460,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{E4694380-2080-4BC6-8827-57DA57D0456F}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{BF58DCA5-60D9-4BB0-BBAB-E9F051CC5D89}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{E4E1F342-2F55-4DB0-8E32-26255C0F4B8A}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{E4E1F342-2F55-4DB0-8E32-26255C0F4B8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>